<commit_message>
adding new files, reports and images
</commit_message>
<xml_diff>
--- a/src/main/java/com/OrangeHRM/qa/testData/OrangeHRM_TestData.xlsx
+++ b/src/main/java/com/OrangeHRM/qa/testData/OrangeHRM_TestData.xlsx
@@ -1,33 +1,43 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mahes\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\My_Automation_Projects\OrangeHRM_Automation_Project\src\main\java\com\OrangeHRM\qa\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E05719EF-25C8-48F5-85BB-7D6E195F93E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A06CC99-1F9E-4FF3-B4F2-45A24EB72881}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Environment" sheetId="1" r:id="rId1"/>
-    <sheet name="LoginPage" sheetId="2" r:id="rId2"/>
-    <sheet name="HomePage" sheetId="3" r:id="rId3"/>
+    <sheet name="AddEmployee" sheetId="4" r:id="rId2"/>
+    <sheet name="LoginPage" sheetId="2" r:id="rId3"/>
+    <sheet name="HomePage" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
   <si>
     <t>Environment</t>
   </si>
@@ -51,13 +61,79 @@
   </si>
   <si>
     <t>admin123</t>
+  </si>
+  <si>
+    <t>Mahesh</t>
+  </si>
+  <si>
+    <t>Samba</t>
+  </si>
+  <si>
+    <t>Kiran</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>Goud</t>
+  </si>
+  <si>
+    <t>Uppala</t>
+  </si>
+  <si>
+    <t>Chiramana</t>
+  </si>
+  <si>
+    <t>Pavan</t>
+  </si>
+  <si>
+    <t>Nadavala</t>
+  </si>
+  <si>
+    <t>Keshav</t>
+  </si>
+  <si>
+    <t>Chenna</t>
+  </si>
+  <si>
+    <t>KiranChiramana</t>
+  </si>
+  <si>
+    <t>MaheshGoud</t>
+  </si>
+  <si>
+    <t>SambaUppala</t>
+  </si>
+  <si>
+    <t>PavanNadavala</t>
+  </si>
+  <si>
+    <t>KeshavChenna</t>
+  </si>
+  <si>
+    <t>Mahesh@Goud123</t>
+  </si>
+  <si>
+    <t>Samba@Uppala123</t>
+  </si>
+  <si>
+    <t>Kiran@Chiramana123</t>
+  </si>
+  <si>
+    <t>Pavan@Nadavala123</t>
+  </si>
+  <si>
+    <t>Keshav@Chenna123</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -73,8 +149,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -84,6 +168,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -115,7 +205,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -127,6 +217,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -407,10 +498,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -419,36 +510,48 @@
     <col min="2" max="2" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C1" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C3" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>7</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -458,6 +561,112 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0D21885-11FE-4C7E-BE4D-B91DD538E949}">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.88671875" customWidth="1"/>
+    <col min="2" max="2" width="10.109375" customWidth="1"/>
+    <col min="3" max="3" width="10.5546875" customWidth="1"/>
+    <col min="4" max="4" width="19.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6BA20A2-F0B1-4908-BE41-D500886ADA28}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -471,7 +680,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACEEE351-5072-46C5-B680-134914D0E6BF}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>